<commit_message>
2140 en 2150 toegevoegd
</commit_message>
<xml_diff>
--- a/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.12.xlsx
+++ b/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCD7779-8D52-4669-A909-9D27DB4C3E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E84ACCA-F898-4076-B04F-FF02ED58A0E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TPOD" sheetId="12" r:id="rId1"/>
@@ -2718,7 +2718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2893,35 +2893,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{DD73F50D-CE68-4CBD-BD67-3376699AD112}"/>
   </cellStyles>
-  <dxfs count="329">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="327">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -6518,8 +6495,8 @@
   <dimension ref="A1:AB120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13745,7 +13722,7 @@
       <c r="A90" s="36" t="s">
         <v>703</v>
       </c>
-      <c r="B90" s="66" t="s">
+      <c r="B90" s="58" t="s">
         <v>766</v>
       </c>
       <c r="C90" s="50" t="s">
@@ -13824,7 +13801,7 @@
       <c r="A91" s="36" t="s">
         <v>703</v>
       </c>
-      <c r="B91" s="66" t="s">
+      <c r="B91" s="58" t="s">
         <v>767</v>
       </c>
       <c r="C91" s="50" t="s">
@@ -14076,77 +14053,77 @@
   </sheetData>
   <autoFilter ref="A1:Y91" xr:uid="{9EE4866E-E834-4DB8-9ED6-70561D41353B}"/>
   <conditionalFormatting sqref="M63 O63 Q63 S63 U63 W63 Y63 B2:Y49 A2:A91">
-    <cfRule type="containsText" dxfId="328" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="326" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N63">
-    <cfRule type="containsText" dxfId="327" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="325" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63">
-    <cfRule type="containsText" dxfId="326" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="324" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:K64">
-    <cfRule type="containsText" dxfId="325" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="323" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1">
-    <cfRule type="containsText" dxfId="324" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="322" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R63">
-    <cfRule type="containsText" dxfId="323" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="321" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T63">
-    <cfRule type="containsText" dxfId="322" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="320" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V63">
-    <cfRule type="containsText" dxfId="321" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="319" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",V63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X63">
-    <cfRule type="containsText" dxfId="320" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="318" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",X63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P63">
-    <cfRule type="containsText" dxfId="319" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="317" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="318" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="316" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="containsText" dxfId="317" priority="44" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="315" priority="44" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="containsText" dxfId="316" priority="43" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="314" priority="43" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z49">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="313" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Z2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z64">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="312" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Z64)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37428,1562 +37405,1562 @@
   </sheetData>
   <autoFilter ref="A1:V343" xr:uid="{C54AF10E-E059-4F84-9C3A-10A5CBE61918}"/>
   <conditionalFormatting sqref="C180:H208 D209:D263 E209:E261 C209:C249 F209:H262 G283:H302 A28:A29 A1:E27 A152:H152 A30:F48 A59:H126 G1:V1 G2:H48 J2:J48 J59:J126 L59:L126 L2:L48 N2:N48 N59:N126 J152 J180:J262 L180:L262 L152 N152 N180:N262 P180:P262 P152 P59:P126 P2:P48 R2:R48 R59:R126 R152 T152 T59:T126 T2:T48 V2:V48 V59:V126 V152 P283:P302 N283:N302 L283:L302 J283:J302">
-    <cfRule type="containsText" dxfId="313" priority="351" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="311" priority="351" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E29 F1:F29">
-    <cfRule type="containsText" dxfId="312" priority="350" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="310" priority="350" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="311" priority="349" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="309" priority="349" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="310" priority="348" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="308" priority="348" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C283:C302">
-    <cfRule type="containsText" dxfId="309" priority="333" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="307" priority="333" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C283)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D283:F302">
-    <cfRule type="containsText" dxfId="308" priority="347" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="306" priority="347" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D283)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C262:C263 E262">
-    <cfRule type="containsText" dxfId="307" priority="334" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="305" priority="334" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C250">
-    <cfRule type="containsText" dxfId="306" priority="346" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="304" priority="346" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C251">
-    <cfRule type="containsText" dxfId="305" priority="345" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="303" priority="345" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C252">
-    <cfRule type="containsText" dxfId="304" priority="344" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="302" priority="344" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C253">
-    <cfRule type="containsText" dxfId="303" priority="343" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="301" priority="343" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C253)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C254">
-    <cfRule type="containsText" dxfId="302" priority="342" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="300" priority="342" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="301" priority="341" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="299" priority="341" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256">
-    <cfRule type="containsText" dxfId="300" priority="340" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="298" priority="340" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C257">
-    <cfRule type="containsText" dxfId="299" priority="339" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="297" priority="339" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C257)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C258">
-    <cfRule type="containsText" dxfId="298" priority="338" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="296" priority="338" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C259">
-    <cfRule type="containsText" dxfId="297" priority="337" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="295" priority="337" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C259)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C260">
-    <cfRule type="containsText" dxfId="296" priority="336" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="294" priority="336" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C261">
-    <cfRule type="containsText" dxfId="295" priority="335" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="293" priority="335" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E53 G49:H53 J49:J53 L49:L53 N49:N53 P49:P53 R49:R53 T49:T53 V49:V53">
-    <cfRule type="containsText" dxfId="294" priority="327" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="292" priority="327" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F53">
-    <cfRule type="containsText" dxfId="293" priority="326" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="291" priority="326" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:E58 G54:H58 J54:J58 L54:L58 N54:N58 P54:P58 R54:R58 T54:T58 V54:V58">
-    <cfRule type="containsText" dxfId="292" priority="325" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="290" priority="325" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F58">
-    <cfRule type="containsText" dxfId="291" priority="324" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="289" priority="324" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q48 Q59:Q126 Q152">
-    <cfRule type="containsText" dxfId="290" priority="302" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="288" priority="302" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49:Q53">
-    <cfRule type="containsText" dxfId="289" priority="301" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="287" priority="301" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54:Q58">
-    <cfRule type="containsText" dxfId="288" priority="300" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="286" priority="300" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S58">
-    <cfRule type="containsText" dxfId="287" priority="297" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="285" priority="297" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U48 U59:U126 U152">
-    <cfRule type="containsText" dxfId="286" priority="296" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="284" priority="296" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U49:U53">
-    <cfRule type="containsText" dxfId="285" priority="295" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="283" priority="295" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54:U58">
-    <cfRule type="containsText" dxfId="284" priority="294" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="282" priority="294" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q180:Q262 Q283:Q302">
-    <cfRule type="containsText" dxfId="283" priority="289" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="281" priority="289" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48 I59:I126 I152 I180:I262 I283:I302">
-    <cfRule type="containsText" dxfId="282" priority="314" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="280" priority="314" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I53">
-    <cfRule type="containsText" dxfId="281" priority="313" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="279" priority="313" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I58">
-    <cfRule type="containsText" dxfId="280" priority="312" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="278" priority="312" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:K126 K2:K48 K180:K262 K152 K283:K302">
-    <cfRule type="containsText" dxfId="279" priority="311" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="277" priority="311" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="containsText" dxfId="278" priority="310" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="276" priority="310" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:K58">
-    <cfRule type="containsText" dxfId="277" priority="309" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="275" priority="309" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M48 M59:M126 M152 M180:M262 M283:M302">
-    <cfRule type="containsText" dxfId="276" priority="308" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="274" priority="308" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M53">
-    <cfRule type="containsText" dxfId="275" priority="307" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="273" priority="307" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M58">
-    <cfRule type="containsText" dxfId="274" priority="306" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="272" priority="306" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O180:O262 O152 O59:O126 O2:O48 O283:O302">
-    <cfRule type="containsText" dxfId="273" priority="305" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="271" priority="305" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O53">
-    <cfRule type="containsText" dxfId="272" priority="304" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="270" priority="304" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54:O58">
-    <cfRule type="containsText" dxfId="271" priority="303" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="269" priority="303" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S152 S59:S126 S2:S48">
-    <cfRule type="containsText" dxfId="270" priority="299" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="268" priority="299" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S53">
-    <cfRule type="containsText" dxfId="269" priority="298" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="267" priority="298" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V180:V261 T180:T261 T283:T302 V283:V302">
-    <cfRule type="containsText" dxfId="268" priority="293" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="266" priority="293" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U180:U261 U283:U302">
-    <cfRule type="containsText" dxfId="267" priority="292" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="265" priority="292" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S180:S261 S283:S302">
-    <cfRule type="containsText" dxfId="266" priority="291" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="264" priority="291" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R180:R262 R283:R302">
-    <cfRule type="containsText" dxfId="265" priority="290" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="263" priority="290" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F263:H263 J263 L263 N263 P263">
-    <cfRule type="containsText" dxfId="264" priority="288" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="262" priority="288" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E263">
-    <cfRule type="containsText" dxfId="263" priority="287" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="261" priority="287" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q263">
-    <cfRule type="containsText" dxfId="262" priority="278" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="260" priority="278" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I263">
-    <cfRule type="containsText" dxfId="261" priority="286" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="259" priority="286" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K263">
-    <cfRule type="containsText" dxfId="260" priority="285" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="258" priority="285" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M263">
-    <cfRule type="containsText" dxfId="259" priority="284" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="257" priority="284" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O263">
-    <cfRule type="containsText" dxfId="258" priority="283" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="256" priority="283" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K264">
-    <cfRule type="containsText" dxfId="257" priority="272" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="255" priority="272" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M264">
-    <cfRule type="containsText" dxfId="256" priority="271" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="254" priority="271" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O264">
-    <cfRule type="containsText" dxfId="255" priority="270" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="253" priority="270" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R263">
-    <cfRule type="containsText" dxfId="254" priority="279" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="252" priority="279" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D264:D266 D273">
-    <cfRule type="containsText" dxfId="253" priority="277" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="251" priority="277" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C264:C266 C273">
-    <cfRule type="containsText" dxfId="252" priority="276" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="250" priority="276" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F264:H264 J264 L264 N264 P264">
-    <cfRule type="containsText" dxfId="251" priority="275" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="249" priority="275" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E264">
-    <cfRule type="containsText" dxfId="250" priority="274" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="248" priority="274" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q264">
-    <cfRule type="containsText" dxfId="249" priority="265" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="247" priority="265" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I264">
-    <cfRule type="containsText" dxfId="248" priority="273" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="246" priority="273" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V264 T264">
-    <cfRule type="containsText" dxfId="247" priority="269" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="245" priority="269" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U264">
-    <cfRule type="containsText" dxfId="246" priority="268" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="244" priority="268" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S264">
-    <cfRule type="containsText" dxfId="245" priority="267" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="243" priority="267" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R264">
-    <cfRule type="containsText" dxfId="244" priority="266" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="242" priority="266" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S262">
-    <cfRule type="containsText" dxfId="243" priority="255" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="241" priority="255" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U262">
-    <cfRule type="containsText" dxfId="242" priority="254" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="240" priority="254" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U263">
-    <cfRule type="containsText" dxfId="241" priority="251" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="239" priority="251" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T263 V263">
-    <cfRule type="containsText" dxfId="240" priority="253" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="238" priority="253" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T262 V262">
-    <cfRule type="containsText" dxfId="239" priority="256" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="237" priority="256" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S263">
-    <cfRule type="containsText" dxfId="238" priority="252" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="236" priority="252" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S263)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F265:H265 J265 L265 N265 P265">
-    <cfRule type="containsText" dxfId="237" priority="250" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="235" priority="250" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E265">
-    <cfRule type="containsText" dxfId="236" priority="249" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="234" priority="249" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q265">
-    <cfRule type="containsText" dxfId="235" priority="243" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="233" priority="243" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I265">
-    <cfRule type="containsText" dxfId="234" priority="248" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="232" priority="248" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K265">
-    <cfRule type="containsText" dxfId="233" priority="247" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="231" priority="247" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M265">
-    <cfRule type="containsText" dxfId="232" priority="246" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="230" priority="246" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O265">
-    <cfRule type="containsText" dxfId="231" priority="245" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="229" priority="245" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R265">
-    <cfRule type="containsText" dxfId="230" priority="244" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="228" priority="244" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U265">
-    <cfRule type="containsText" dxfId="229" priority="240" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="227" priority="240" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T265 V265">
-    <cfRule type="containsText" dxfId="228" priority="242" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="226" priority="242" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S265">
-    <cfRule type="containsText" dxfId="227" priority="241" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="225" priority="241" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S265)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J266 L266 N266 P266 F266:H266 F273:H273">
-    <cfRule type="containsText" dxfId="226" priority="239" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="224" priority="239" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E266 E273">
-    <cfRule type="containsText" dxfId="225" priority="238" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="223" priority="238" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q266">
-    <cfRule type="containsText" dxfId="224" priority="232" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="222" priority="232" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I266">
-    <cfRule type="containsText" dxfId="223" priority="237" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="221" priority="237" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K266">
-    <cfRule type="containsText" dxfId="222" priority="236" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="220" priority="236" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M266">
-    <cfRule type="containsText" dxfId="221" priority="235" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="219" priority="235" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O266">
-    <cfRule type="containsText" dxfId="220" priority="234" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="218" priority="234" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R266">
-    <cfRule type="containsText" dxfId="219" priority="233" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="217" priority="233" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U266">
-    <cfRule type="containsText" dxfId="218" priority="229" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="216" priority="229" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T266 V266">
-    <cfRule type="containsText" dxfId="217" priority="231" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="215" priority="231" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S266">
-    <cfRule type="containsText" dxfId="216" priority="230" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="214" priority="230" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S266)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J273 L273 N273 P273">
-    <cfRule type="containsText" dxfId="215" priority="228" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="213" priority="228" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q273">
-    <cfRule type="containsText" dxfId="214" priority="222" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="212" priority="222" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I273">
-    <cfRule type="containsText" dxfId="213" priority="227" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="211" priority="227" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K273">
-    <cfRule type="containsText" dxfId="212" priority="226" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="210" priority="226" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M273">
-    <cfRule type="containsText" dxfId="211" priority="225" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="209" priority="225" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O273">
-    <cfRule type="containsText" dxfId="210" priority="224" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="208" priority="224" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R273">
-    <cfRule type="containsText" dxfId="209" priority="223" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="207" priority="223" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U273">
-    <cfRule type="containsText" dxfId="208" priority="219" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="206" priority="219" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T273 V273">
-    <cfRule type="containsText" dxfId="207" priority="221" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="205" priority="221" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S273">
-    <cfRule type="containsText" dxfId="206" priority="220" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="204" priority="220" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D274">
-    <cfRule type="containsText" dxfId="205" priority="218" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="203" priority="218" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C274">
-    <cfRule type="containsText" dxfId="204" priority="217" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="202" priority="217" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F274:H274">
-    <cfRule type="containsText" dxfId="203" priority="216" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="201" priority="216" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E274">
-    <cfRule type="containsText" dxfId="202" priority="215" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="200" priority="215" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J274 L274 N274 P274">
-    <cfRule type="containsText" dxfId="201" priority="214" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="199" priority="214" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q274">
-    <cfRule type="containsText" dxfId="200" priority="208" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="198" priority="208" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I274">
-    <cfRule type="containsText" dxfId="199" priority="213" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="197" priority="213" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K274">
-    <cfRule type="containsText" dxfId="198" priority="212" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="196" priority="212" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M274">
-    <cfRule type="containsText" dxfId="197" priority="211" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="195" priority="211" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O274">
-    <cfRule type="containsText" dxfId="196" priority="210" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="194" priority="210" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R274">
-    <cfRule type="containsText" dxfId="195" priority="209" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="193" priority="209" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U274">
-    <cfRule type="containsText" dxfId="194" priority="205" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="192" priority="205" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T274 V274">
-    <cfRule type="containsText" dxfId="193" priority="207" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="191" priority="207" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S274">
-    <cfRule type="containsText" dxfId="192" priority="206" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="190" priority="206" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S274)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D275">
-    <cfRule type="containsText" dxfId="191" priority="204" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="189" priority="204" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C275">
-    <cfRule type="containsText" dxfId="190" priority="203" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="188" priority="203" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F275:H275">
-    <cfRule type="containsText" dxfId="189" priority="202" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="187" priority="202" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E275">
-    <cfRule type="containsText" dxfId="188" priority="201" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="186" priority="201" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J275 L275 N275 P275">
-    <cfRule type="containsText" dxfId="187" priority="200" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="185" priority="200" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q275">
-    <cfRule type="containsText" dxfId="186" priority="194" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="184" priority="194" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I275">
-    <cfRule type="containsText" dxfId="185" priority="199" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="183" priority="199" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K275">
-    <cfRule type="containsText" dxfId="184" priority="198" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="182" priority="198" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M275">
-    <cfRule type="containsText" dxfId="183" priority="197" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="181" priority="197" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O275">
-    <cfRule type="containsText" dxfId="182" priority="196" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="180" priority="196" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R275">
-    <cfRule type="containsText" dxfId="181" priority="195" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="179" priority="195" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U275">
-    <cfRule type="containsText" dxfId="180" priority="191" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="178" priority="191" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T275 V275">
-    <cfRule type="containsText" dxfId="179" priority="193" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="177" priority="193" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S275">
-    <cfRule type="containsText" dxfId="178" priority="192" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="176" priority="192" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S275)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D276">
-    <cfRule type="containsText" dxfId="177" priority="190" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="175" priority="190" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C276">
-    <cfRule type="containsText" dxfId="176" priority="189" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="174" priority="189" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F276:H276">
-    <cfRule type="containsText" dxfId="175" priority="188" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="173" priority="188" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E276">
-    <cfRule type="containsText" dxfId="174" priority="187" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="172" priority="187" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J276 L276 N276 P276">
-    <cfRule type="containsText" dxfId="173" priority="186" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="171" priority="186" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q276">
-    <cfRule type="containsText" dxfId="172" priority="180" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="170" priority="180" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I276">
-    <cfRule type="containsText" dxfId="171" priority="185" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="169" priority="185" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K276">
-    <cfRule type="containsText" dxfId="170" priority="184" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="168" priority="184" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M276">
-    <cfRule type="containsText" dxfId="169" priority="183" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="167" priority="183" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O276">
-    <cfRule type="containsText" dxfId="168" priority="182" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="166" priority="182" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R276">
-    <cfRule type="containsText" dxfId="167" priority="181" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="165" priority="181" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U276">
-    <cfRule type="containsText" dxfId="166" priority="177" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="164" priority="177" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T276 V276">
-    <cfRule type="containsText" dxfId="165" priority="179" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="163" priority="179" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S276">
-    <cfRule type="containsText" dxfId="164" priority="178" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="162" priority="178" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S276)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D277">
-    <cfRule type="containsText" dxfId="163" priority="176" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="161" priority="176" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C277">
-    <cfRule type="containsText" dxfId="162" priority="175" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="160" priority="175" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F277:H277">
-    <cfRule type="containsText" dxfId="161" priority="174" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="159" priority="174" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E277">
-    <cfRule type="containsText" dxfId="160" priority="173" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="158" priority="173" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J277 L277 N277 P277">
-    <cfRule type="containsText" dxfId="159" priority="172" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="157" priority="172" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q277">
-    <cfRule type="containsText" dxfId="158" priority="166" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="156" priority="166" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I277">
-    <cfRule type="containsText" dxfId="157" priority="171" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="155" priority="171" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K277">
-    <cfRule type="containsText" dxfId="156" priority="170" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="154" priority="170" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M277">
-    <cfRule type="containsText" dxfId="155" priority="169" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="153" priority="169" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O277">
-    <cfRule type="containsText" dxfId="154" priority="168" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="152" priority="168" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R277">
-    <cfRule type="containsText" dxfId="153" priority="167" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="151" priority="167" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U277">
-    <cfRule type="containsText" dxfId="152" priority="163" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="150" priority="163" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T277 V277">
-    <cfRule type="containsText" dxfId="151" priority="165" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="149" priority="165" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S277">
-    <cfRule type="containsText" dxfId="150" priority="164" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="148" priority="164" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S277)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U268">
-    <cfRule type="containsText" dxfId="149" priority="67" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="147" priority="67" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U267">
-    <cfRule type="containsText" dxfId="148" priority="80" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="146" priority="80" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U270">
-    <cfRule type="containsText" dxfId="147" priority="41" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="145" priority="41" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D278">
-    <cfRule type="containsText" dxfId="146" priority="162" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="144" priority="162" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C278">
-    <cfRule type="containsText" dxfId="145" priority="161" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="143" priority="161" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F278:H278">
-    <cfRule type="containsText" dxfId="144" priority="160" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="142" priority="160" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E278">
-    <cfRule type="containsText" dxfId="143" priority="159" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="141" priority="159" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J278 L278 N278 P278">
-    <cfRule type="containsText" dxfId="142" priority="158" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="140" priority="158" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q278">
-    <cfRule type="containsText" dxfId="141" priority="152" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="139" priority="152" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I278">
-    <cfRule type="containsText" dxfId="140" priority="157" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="138" priority="157" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K278">
-    <cfRule type="containsText" dxfId="139" priority="156" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="137" priority="156" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M278">
-    <cfRule type="containsText" dxfId="138" priority="155" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="136" priority="155" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O278">
-    <cfRule type="containsText" dxfId="137" priority="154" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="135" priority="154" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R278">
-    <cfRule type="containsText" dxfId="136" priority="153" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="134" priority="153" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U278">
-    <cfRule type="containsText" dxfId="135" priority="149" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="133" priority="149" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T278 V278">
-    <cfRule type="containsText" dxfId="134" priority="151" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="132" priority="151" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S278">
-    <cfRule type="containsText" dxfId="133" priority="150" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="131" priority="150" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D279">
-    <cfRule type="containsText" dxfId="132" priority="148" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="130" priority="148" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C279">
-    <cfRule type="containsText" dxfId="131" priority="147" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="129" priority="147" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F279:H279">
-    <cfRule type="containsText" dxfId="130" priority="146" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="128" priority="146" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E279">
-    <cfRule type="containsText" dxfId="129" priority="145" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="127" priority="145" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J279 L279 N279 P279">
-    <cfRule type="containsText" dxfId="128" priority="144" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="126" priority="144" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q279">
-    <cfRule type="containsText" dxfId="127" priority="138" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="125" priority="138" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I279">
-    <cfRule type="containsText" dxfId="126" priority="143" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="124" priority="143" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K279">
-    <cfRule type="containsText" dxfId="125" priority="142" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="123" priority="142" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M279">
-    <cfRule type="containsText" dxfId="124" priority="141" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="122" priority="141" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O279">
-    <cfRule type="containsText" dxfId="123" priority="140" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="121" priority="140" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R279">
-    <cfRule type="containsText" dxfId="122" priority="139" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="120" priority="139" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U279">
-    <cfRule type="containsText" dxfId="121" priority="135" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="119" priority="135" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T279 V279">
-    <cfRule type="containsText" dxfId="120" priority="137" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="118" priority="137" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S279">
-    <cfRule type="containsText" dxfId="119" priority="136" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="117" priority="136" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S279)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D280">
-    <cfRule type="containsText" dxfId="118" priority="134" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="116" priority="134" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C280">
-    <cfRule type="containsText" dxfId="117" priority="133" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="115" priority="133" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F280:H280">
-    <cfRule type="containsText" dxfId="116" priority="132" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="114" priority="132" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E280">
-    <cfRule type="containsText" dxfId="115" priority="131" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="113" priority="131" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J280 L280 N280 P280">
-    <cfRule type="containsText" dxfId="114" priority="130" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="112" priority="130" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q280">
-    <cfRule type="containsText" dxfId="113" priority="124" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="111" priority="124" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I280">
-    <cfRule type="containsText" dxfId="112" priority="129" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="110" priority="129" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K280">
-    <cfRule type="containsText" dxfId="111" priority="128" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="109" priority="128" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M280">
-    <cfRule type="containsText" dxfId="110" priority="127" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="108" priority="127" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O280">
-    <cfRule type="containsText" dxfId="109" priority="126" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="107" priority="126" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R280">
-    <cfRule type="containsText" dxfId="108" priority="125" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="106" priority="125" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U280">
-    <cfRule type="containsText" dxfId="107" priority="121" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="105" priority="121" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T280 V280">
-    <cfRule type="containsText" dxfId="106" priority="123" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="104" priority="123" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S280">
-    <cfRule type="containsText" dxfId="105" priority="122" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="103" priority="122" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D281">
-    <cfRule type="containsText" dxfId="104" priority="120" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="102" priority="120" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C281">
-    <cfRule type="containsText" dxfId="103" priority="119" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="101" priority="119" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F281:H281">
-    <cfRule type="containsText" dxfId="102" priority="118" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="100" priority="118" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E281">
-    <cfRule type="containsText" dxfId="101" priority="117" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="99" priority="117" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J281 L281 N281 P281">
-    <cfRule type="containsText" dxfId="100" priority="116" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="98" priority="116" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q281">
-    <cfRule type="containsText" dxfId="99" priority="110" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="97" priority="110" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I281">
-    <cfRule type="containsText" dxfId="98" priority="115" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="96" priority="115" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K281">
-    <cfRule type="containsText" dxfId="97" priority="114" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="95" priority="114" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M281">
-    <cfRule type="containsText" dxfId="96" priority="113" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="94" priority="113" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O281">
-    <cfRule type="containsText" dxfId="95" priority="112" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="93" priority="112" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R281">
-    <cfRule type="containsText" dxfId="94" priority="111" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="92" priority="111" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U281">
-    <cfRule type="containsText" dxfId="93" priority="107" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="91" priority="107" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T281 V281">
-    <cfRule type="containsText" dxfId="92" priority="109" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="90" priority="109" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S281">
-    <cfRule type="containsText" dxfId="91" priority="108" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="89" priority="108" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D268">
-    <cfRule type="containsText" dxfId="90" priority="79" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="88" priority="79" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C268">
-    <cfRule type="containsText" dxfId="89" priority="78" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="87" priority="78" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J268 L268 N268 P268 F268:H268">
-    <cfRule type="containsText" dxfId="88" priority="77" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="86" priority="77" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E268">
-    <cfRule type="containsText" dxfId="87" priority="76" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="85" priority="76" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q268">
-    <cfRule type="containsText" dxfId="86" priority="70" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="84" priority="70" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I268">
-    <cfRule type="containsText" dxfId="85" priority="75" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="83" priority="75" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K268">
-    <cfRule type="containsText" dxfId="84" priority="74" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="82" priority="74" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M268">
-    <cfRule type="containsText" dxfId="83" priority="73" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="81" priority="73" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O268">
-    <cfRule type="containsText" dxfId="82" priority="72" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="80" priority="72" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R268">
-    <cfRule type="containsText" dxfId="81" priority="71" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="79" priority="71" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T268 V268">
-    <cfRule type="containsText" dxfId="80" priority="69" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="78" priority="69" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S268">
-    <cfRule type="containsText" dxfId="79" priority="68" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="77" priority="68" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D267">
-    <cfRule type="containsText" dxfId="78" priority="92" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="76" priority="92" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267">
-    <cfRule type="containsText" dxfId="77" priority="91" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="75" priority="91" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J267 L267 N267 P267 F267:H267">
-    <cfRule type="containsText" dxfId="76" priority="90" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="74" priority="90" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E267">
-    <cfRule type="containsText" dxfId="75" priority="89" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="73" priority="89" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q267">
-    <cfRule type="containsText" dxfId="74" priority="83" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="72" priority="83" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I267">
-    <cfRule type="containsText" dxfId="73" priority="88" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="71" priority="88" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K267">
-    <cfRule type="containsText" dxfId="72" priority="87" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="70" priority="87" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M267">
-    <cfRule type="containsText" dxfId="71" priority="86" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="69" priority="86" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O267">
-    <cfRule type="containsText" dxfId="70" priority="85" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="85" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R267">
-    <cfRule type="containsText" dxfId="69" priority="84" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="84" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T267 V267">
-    <cfRule type="containsText" dxfId="68" priority="82" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="66" priority="82" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S267">
-    <cfRule type="containsText" dxfId="67" priority="81" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="65" priority="81" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U269">
-    <cfRule type="containsText" dxfId="66" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="64" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D269">
-    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C269">
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="62" priority="65" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J269 L269 N269 P269 F269:H269">
-    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="61" priority="64" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E269">
-    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q269">
-    <cfRule type="containsText" dxfId="61" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I269">
-    <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K269">
-    <cfRule type="containsText" dxfId="59" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M269">
-    <cfRule type="containsText" dxfId="58" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O269">
-    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R269">
-    <cfRule type="containsText" dxfId="56" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T269 V269">
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S269">
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S269)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D270">
-    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C270">
-    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J270 L270 N270 P270 F270:H270">
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E270">
-    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q270">
-    <cfRule type="containsText" dxfId="49" priority="44" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="44" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I270">
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K270">
-    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M270">
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O270">
-    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R270">
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T270 V270">
-    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S270">
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S270)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U271">
-    <cfRule type="containsText" dxfId="41" priority="28" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="28" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D271">
-    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C271">
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J271 L271 N271 P271 F271:H271">
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E271">
-    <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q271">
-    <cfRule type="containsText" dxfId="36" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I271">
-    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K271">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M271">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O271">
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R271">
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T271 V271">
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S271">
-    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S271)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U272">
-    <cfRule type="containsText" dxfId="28" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D272">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C272">
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J272 L272 N272 P272 F272:H272">
-    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E272">
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q272">
-    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I272">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K272">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M272">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O272">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R272">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T272 V272">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S272">
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D282">
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F282:H282">
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E282">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J282 L282 N282 P282">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q282">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I282">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K282">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M282">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O282">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R282">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U282">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T282 V282">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S282">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S282)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>